<commit_message>
Version 3: Agregar texto a 2 archivos.
</commit_message>
<xml_diff>
--- a/ArchivoDos.xlsx
+++ b/ArchivoDos.xlsx
@@ -18,11 +18,27 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>AGREGANDO CAMBIOS AL REPOSITORIO</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -49,8 +65,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -69,7 +88,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +133,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +168,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +350,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:I2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>